<commit_message>
Excel sheet error handling
</commit_message>
<xml_diff>
--- a/sample_stock_data.xlsx
+++ b/sample_stock_data.xlsx
@@ -73,7 +73,7 @@
     <t xml:space="preserve">  11:05:00</t>
   </si>
   <si>
-    <t xml:space="preserve">  11:10:00</t>
+    <t xml:space="preserve"> 23:10:00</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="A11:E11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>